<commit_message>
Update Signup test case
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L e n o v o\Documents\My Documents\Test Cases\HelaFix\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L e n o v o\Documents\My Documents\Test Cases\HelaFix\QA-Testing-Project-HelaFix-Mobile-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F703F4E-D123-4E5D-A9D9-9620FF939137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A9D433-C117-4A93-9150-B861256EA512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{37C3E088-A2BC-493D-8AA3-73211FA0C21C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{37C3E088-A2BC-493D-8AA3-73211FA0C21C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SignUp" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="74">
   <si>
     <t>Project Name</t>
   </si>
@@ -426,9 +427,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -440,6 +438,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85A5934-7E8A-4804-A8E0-C39FC8F2C93D}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -864,370 +865,370 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="12" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="12" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H16" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="H19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1238,4 +1239,464 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE9CD41-F367-4F17-97F0-9226E6996871}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="12" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="1:16" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="1:16" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test Cases for SignIn page
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L e n o v o\Documents\My Documents\Test Cases\HelaFix\QA-Testing-Project-HelaFix-Mobile-App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22177023-F345-45D9-89DB-D2AFBCF17E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C859442-5C59-438D-A97C-F23D4F304398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{37C3E088-A2BC-493D-8AA3-73211FA0C21C}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="SignIn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="111">
   <si>
     <t>Project Name</t>
   </si>
@@ -353,6 +353,128 @@
   </si>
   <si>
     <t>User navigate to Home screen.</t>
+  </si>
+  <si>
+    <t>Valid Login</t>
+  </si>
+  <si>
+    <t>Verify user can log in with valid credentials</t>
+  </si>
+  <si>
+    <t>Email: user@example.com
+Password: CorrectPass123</t>
+  </si>
+  <si>
+    <t>User is redirected to homepage</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>Check error for wrong password</t>
+  </si>
+  <si>
+    <t>1. Go to login page
+2. Enter valid email and wrong password
+3. Click 'Sign In'</t>
+  </si>
+  <si>
+    <t>Email: user@example.com
+Password: WrongPass</t>
+  </si>
+  <si>
+    <t>Error message: 'Incorrect password'</t>
+  </si>
+  <si>
+    <t>Invalid Email Format</t>
+  </si>
+  <si>
+    <t>Validate system for incorrect email format</t>
+  </si>
+  <si>
+    <t>1. Enter email without '@'
+2. Attempt login</t>
+  </si>
+  <si>
+    <t>Email: userexample.com</t>
+  </si>
+  <si>
+    <t>Validation error displayed</t>
+  </si>
+  <si>
+    <t>Empty Fields</t>
+  </si>
+  <si>
+    <t>Verify login fails with empty fields</t>
+  </si>
+  <si>
+    <t>1. Click 'Sign In' without entering credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email: 
+Password: </t>
+  </si>
+  <si>
+    <t>Error: 'Fields required'</t>
+  </si>
+  <si>
+    <t>No login attempt made</t>
+  </si>
+  <si>
+    <t>1. Click on 'Sign In'
+2. Enter valid email and password
+3. Click 'Sign In'</t>
+  </si>
+  <si>
+    <t>Customer should signin successfully with the system</t>
+  </si>
+  <si>
+    <t>Create account option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify whether the Create account option is working </t>
+  </si>
+  <si>
+    <t>1. Go to login page
+2. Press create account</t>
+  </si>
+  <si>
+    <t>User is redirected to SignUp page</t>
+  </si>
+  <si>
+    <t>Sign up page is displayed</t>
+  </si>
+  <si>
+    <t>Login with google</t>
+  </si>
+  <si>
+    <t>1. Go to login page
+2. Press Login with google                      3. Select one account</t>
+  </si>
+  <si>
+    <t>Google sign in failed</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>pop up error message</t>
+  </si>
+  <si>
+    <t>Login as Service Provider</t>
+  </si>
+  <si>
+    <t>Verify service provider login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to login page
+2. Scroll to " Are you having service provider account?"                   3. Press Log Now          </t>
+  </si>
+  <si>
+    <t>Redirect to Provider Login</t>
+  </si>
+  <si>
+    <t>Provider login</t>
   </si>
 </sst>
 </file>
@@ -778,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85A5934-7E8A-4804-A8E0-C39FC8F2C93D}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1243,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE9CD41-F367-4F17-97F0-9226E6996871}">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:J20"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1332,7 +1454,9 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -1341,7 +1465,9 @@
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -1350,7 +1476,9 @@
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -1387,17 +1515,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+    <row r="13" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
@@ -1405,17 +1553,37 @@
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+    <row r="14" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -1423,17 +1591,37 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+    <row r="15" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -1441,17 +1629,37 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
@@ -1459,17 +1667,37 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+    <row r="17" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -1477,17 +1705,34 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+    <row r="18" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>105</v>
+      </c>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -1495,17 +1740,37 @@
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+    <row r="19" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -1513,30 +1778,13 @@
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>